<commit_message>
Updated documentation folder, now it contains PULP instead of PULPISSIMO
</commit_message>
<xml_diff>
--- a/doc/Pulp_configuration.xlsx
+++ b/doc/Pulp_configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">1.0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">blabla</t>
+    <t xml:space="preserve">First PULP Release</t>
   </si>
   <si>
     <t xml:space="preserve">Rel1.0.0</t>
@@ -4662,17 +4662,17 @@
   </sheetPr>
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4869,7 +4869,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4884,18 +4884,18 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.7004048582996"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.24696356275304"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="64.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5122,10 +5122,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Pagina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5137,18 +5137,18 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="56.9878542510121"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.35627530364373"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="38.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="56.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5230,7 +5230,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5243,21 +5243,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65536"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="146" width="45.9554655870445"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="33.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="146" width="45.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6024,10 +6024,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6037,24 +6037,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K65536"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="146" width="45.9554655870445"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="33.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="146" width="45.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="42.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6580,10 +6580,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6595,18 +6595,18 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="33.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="38.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7113,10 +7113,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -7128,18 +7128,18 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="44.668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="33.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7642,10 +7642,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -7657,16 +7657,16 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.1255060728745"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.35627530364373"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7775,7 +7775,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7790,17 +7790,17 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.35627530364373"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8121,7 +8121,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8136,19 +8136,19 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.81781376518219"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.35627530364373"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8789,7 +8789,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8804,16 +8804,16 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.35627530364373"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9022,7 +9022,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9037,17 +9037,17 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9104,7 +9104,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9119,17 +9119,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1023" min="5" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="5" style="0" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9163,10 +9163,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9178,32 +9178,32 @@
   </sheetPr>
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C93" activeCellId="0" sqref="C93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="35" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="35" width="9"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="35" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="35" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="35" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="36" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="35" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="35" width="6.31983805668016"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="35" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.24696356275304"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="35" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="35" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="35" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="35" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="35" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="36" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="35" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="35" width="6.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="35" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.24"/>
   </cols>
   <sheetData>
     <row r="1" s="36" customFormat="true" ht="72.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13860,10 +13860,10 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -13875,26 +13875,26 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="35" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="35" width="61.5951417004049"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="35" width="62.8785425101215"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.24696356275304"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="33.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="21.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="35" width="27.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="35" width="61.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="35" width="62.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15304,10 +15304,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -15319,15 +15319,15 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="38.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15605,10 +15605,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -15620,17 +15620,17 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="35" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.35627530364373"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="35" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15748,7 +15748,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -15763,33 +15763,33 @@
   </sheetPr>
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="35" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.67611336032389"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="35" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="45" customFormat="true" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20110,7 +20110,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -20125,18 +20125,18 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.5951417004049"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6356275303644"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.24696356275304"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20344,10 +20344,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Pagina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>